<commit_message>
Trying fix lab 3
</commit_message>
<xml_diff>
--- a/Lab3.xlsx
+++ b/Lab3.xlsx
@@ -779,10 +779,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C2" t="n">
-        <v>4831</v>
+        <v>4792</v>
       </c>
     </row>
     <row r="3" ht="192" customHeight="1">

</xml_diff>